<commit_message>
update lunyx less 10 11 12
</commit_message>
<xml_diff>
--- a/training_linux.xlsx
+++ b/training_linux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nerom\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4CC5DE-7D68-4043-8D12-9D137D239F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37B732-09CD-4E5F-B77C-18CB8CF587D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="150" windowWidth="24630" windowHeight="18495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="1815" windowWidth="18285" windowHeight="18480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Базовая инфа" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="598">
   <si>
     <t>Название команды</t>
   </si>
@@ -5591,16 +5591,972 @@
       <t>git checkout -b windows origin/windows(Нужная ветка)</t>
     </r>
   </si>
+  <si>
+    <t>etc/groups</t>
+  </si>
+  <si>
+    <t>Там будет индивидуальный номер который присвоен группе</t>
+  </si>
+  <si>
+    <t>где находится все группы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">присвоить пользователю группу </t>
+  </si>
+  <si>
+    <t>etc/passwd</t>
+  </si>
+  <si>
+    <t>доступ к файлу или папке</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дать право на файл - папку </t>
+  </si>
+  <si>
+    <t>присвоение доступа к файлу</t>
+  </si>
+  <si>
+    <t>chown имя пользователя:имя группы файл</t>
+  </si>
+  <si>
+    <t>в второй строчке числовых индификаторов меняем человеку группу</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - право на чтение. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>w 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- право на запись. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - право на исполнение файла</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">без </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> действия с файлом никакие не возможн</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">chmod </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> разрешение для владельца)(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>разрешение для группы)(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> разрешение для всех остальных)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">пример: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chmod 744 file.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    таким образом все сотальные кроме владельца смогут просмотривать файл но не открывать его в редакторе</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>если нужно присвоить доступ к файлу только группе пишем так</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chown :group file.txt</t>
+    </r>
+  </si>
+  <si>
+    <t>РАСШИРЕННЫЕ ПРАВА ДОСТУПА</t>
+  </si>
+  <si>
+    <t>sticky bit</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">что установить такую возможность нужно добавить нужную цифру без остальными </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">chmod </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>777 test.txt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>suid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> даёт право пользователю повысить свой уровень прав до уровня владельца файла</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sgid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>тоже самое только доступ разрешается группе пользователей</t>
+    </r>
+  </si>
+  <si>
+    <t>Только пользователь создавший файл сможет удалить их в данной дериктории</t>
+  </si>
+  <si>
+    <t>chmod 2777 test.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Так же можно добавить пользователя в группу командой </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usermod -a -G namegroup user</t>
+    </r>
+  </si>
+  <si>
+    <t>https://help.ubuntu.ru/wiki/стандартные_права_unix</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chmod -R 777</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> установит права на каталог и на все объекты</t>
+    </r>
+  </si>
+  <si>
+    <t>Просмотр доступа файла НЕОБЫЧНО</t>
+  </si>
+  <si>
+    <t>getfacl имя файла</t>
+  </si>
+  <si>
+    <t>можно добавить право на файл конкректному человеку</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setfacl -m u:name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rw</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> какие именно права) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+  </si>
+  <si>
+    <t>что бы отменить доступ к файлу юзера</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>setfacl -b имя</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>не на всех ОС работает</t>
+  </si>
+  <si>
+    <t>yum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">поиск </t>
+  </si>
+  <si>
+    <t>Установка программ из репозитория</t>
+  </si>
+  <si>
+    <t>yum search (название)</t>
+  </si>
+  <si>
+    <t>на центос</t>
+  </si>
+  <si>
+    <t>аналог на убунтум apt</t>
+  </si>
+  <si>
+    <t>Стандартные потоки ввода/вывода</t>
+  </si>
+  <si>
+    <t>STDIN -&lt;-0</t>
+  </si>
+  <si>
+    <t>STDOUT -&gt;-1</t>
+  </si>
+  <si>
+    <t>STDEER-2&gt;-2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">пример: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cat testfile.txt &gt; infotext.tx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">t                                          ВАЖНО: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЕСЛИ МЫ ХОТИМ ЧТО БЫ ИНФА ДОПОЛНЯЛАСЬ ТО СТАВИМ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">чем мы вводим данные - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>клавиатура</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Куда выводится информация - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>терминал</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Куда выводится </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ошибки - терминал</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Проще говоря функция &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>перенаправит всю инфу которая выведется в терминале в файл который мы укажем</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>если его нет то  он его создаст, но если есть то система его перезапишет</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Предположим у нас есть файл test1.txt и создать ещё один фийл с такой же инфой</t>
+  </si>
+  <si>
+    <t>cat &gt; test2.txt &lt; test1.txt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Проще говоря мы перенаправили </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в новосозданный файл </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test.txt</t>
+    </r>
+  </si>
+  <si>
+    <t>Все возможные ошибки при выполнении действия  можно записать в отдельный файл</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">например у нас есть файл </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test1, test2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cat test3 2&gt; errortest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">              2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>создастся errortest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>и в нём будет ошибка</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, что такого файла нет</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Запуск программы в фоновом режиме </t>
+  </si>
+  <si>
+    <r>
+      <t>В конце строки добавить</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp;</t>
+    </r>
+  </si>
+  <si>
+    <t>Что бы инфа программ в фоновом режиме не лилась в терминал мы можем пустить поток данных в файл и в конце обьеденив ошибки с ни же</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cat test1 test2 &gt; logs1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2&gt;&amp;1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Получается что данный с файла test1 и test2 попадают в новосозданный logs1 ,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> а ошибки  обьеденятся с первым потоком и зальются туда же</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, запустившись всё в фоновом режиме</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Пример запуска фаерфокса: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>firefox &gt; logs1 2&gt;&amp;1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">p.s. Если мы не знаем что за тип файла у нас </t>
+  </si>
+  <si>
+    <t>file namefile</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ASCII text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   это просто текстовый файл</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5737,8 +6693,32 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5799,6 +6779,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5811,26 +6797,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5839,10 +6825,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -5859,7 +6845,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -5872,46 +6858,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5922,43 +6925,43 @@
   <dxfs count="18">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -7968,18 +8971,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8FD92801-A738-4E97-9685-616EECEC3946}" name="Таблица3" displayName="Таблица3" ref="A1:I41" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
-  <autoFilter ref="A1:I41" xr:uid="{8FD92801-A738-4E97-9685-616EECEC3946}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8FD92801-A738-4E97-9685-616EECEC3946}" name="Таблица3" displayName="Таблица3" ref="A1:I65" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I65" xr:uid="{8FD92801-A738-4E97-9685-616EECEC3946}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1626E174-C694-4FFF-8777-E9762AB1CEC2}" name="Название" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4896455F-2026-4CE1-9950-452163BD0B0A}" name="Структура" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{56504F2D-3058-4F20-BEFC-F5A809469C44}" name="Описание" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{59C03D0A-6E69-47AE-952D-194C080DF02D}" name="Пример1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{3E6FC407-BE89-402A-82F5-D387E3BCA1C4}" name="Пример 2" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{8EC2D2B2-3979-4CFF-B0AF-D113D8D3A33E}" name="Результат" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{B8B83DB3-8636-42D5-93F3-5A59C4C57874}" name="Комментарий 1" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{78064B2D-D083-4483-AE6A-844A50D96135}" name="Комментарий 2" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F4B7C10D-0065-4052-BA24-9E5296111374}" name="Коментарий 3" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1626E174-C694-4FFF-8777-E9762AB1CEC2}" name="Название" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{4896455F-2026-4CE1-9950-452163BD0B0A}" name="Структура" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{56504F2D-3058-4F20-BEFC-F5A809469C44}" name="Описание" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{59C03D0A-6E69-47AE-952D-194C080DF02D}" name="Пример1" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{3E6FC407-BE89-402A-82F5-D387E3BCA1C4}" name="Пример 2" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{8EC2D2B2-3979-4CFF-B0AF-D113D8D3A33E}" name="Результат" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{B8B83DB3-8636-42D5-93F3-5A59C4C57874}" name="Комментарий 1" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{78064B2D-D083-4483-AE6A-844A50D96135}" name="Комментарий 2" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{F4B7C10D-0065-4052-BA24-9E5296111374}" name="Коментарий 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8197,7 +9200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
@@ -10828,10 +11831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8922A16-1323-425E-A295-6954513D6A12}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10886,25 +11889,25 @@
       <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>461</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="36"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="34" t="s">
         <v>451</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -10921,7 +11924,7 @@
       <c r="A4" s="28" t="s">
         <v>464</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="34" t="s">
         <v>436</v>
       </c>
       <c r="C4" s="29" t="s">
@@ -10938,7 +11941,7 @@
       <c r="A5" s="29" t="s">
         <v>529</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="34" t="s">
         <v>438</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -10955,7 +11958,7 @@
       <c r="A6" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="34" t="s">
         <v>441</v>
       </c>
       <c r="C6" s="28"/>
@@ -10970,7 +11973,7 @@
       <c r="A7" s="28" t="s">
         <v>466</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="34" t="s">
         <v>467</v>
       </c>
       <c r="C7" s="28"/>
@@ -10985,7 +11988,7 @@
       <c r="A8" s="28" t="s">
         <v>468</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="34" t="s">
         <v>469</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -11002,7 +12005,7 @@
       <c r="A9" s="28" t="s">
         <v>471</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="34" t="s">
         <v>446</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -11048,25 +12051,25 @@
       <c r="I11" s="28"/>
     </row>
     <row r="12" spans="1:19" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>478</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>479</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="33" t="s">
         <v>480</v>
       </c>
       <c r="C13" s="29" t="s">
@@ -11156,16 +12159,16 @@
       <c r="B18" s="29" t="s">
         <v>515</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>517</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>518</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>519</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
@@ -11174,7 +12177,7 @@
       <c r="A19" s="29" t="s">
         <v>488</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="34" t="s">
         <v>188</v>
       </c>
       <c r="C19" s="28"/>
@@ -11195,7 +12198,7 @@
       <c r="C20" s="29" t="s">
         <v>490</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="34" t="s">
         <v>491</v>
       </c>
       <c r="E20" s="29" t="s">
@@ -11204,7 +12207,7 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="40" t="s">
         <v>492</v>
       </c>
     </row>
@@ -11212,7 +12215,7 @@
       <c r="A21" s="29" t="s">
         <v>493</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
@@ -11240,10 +12243,10 @@
       <c r="A23" s="29" t="s">
         <v>496</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="34" t="s">
         <v>497</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="34" t="s">
         <v>498</v>
       </c>
       <c r="D23" s="28"/>
@@ -11257,7 +12260,7 @@
       <c r="A24" s="29" t="s">
         <v>499</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="34" t="s">
         <v>500</v>
       </c>
       <c r="C24" s="28"/>
@@ -11355,23 +12358,23 @@
       <c r="I30" s="28"/>
     </row>
     <row r="31" spans="1:9" s="26" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="32" t="s">
         <v>503</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
         <v>504</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="34" t="s">
         <v>505</v>
       </c>
       <c r="C32" s="28"/>
@@ -11382,10 +12385,16 @@
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>533</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>534</v>
+      </c>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
@@ -11393,21 +12402,35 @@
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
+    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>536</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>537</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>558</v>
+      </c>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>538</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>543</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>544</v>
+      </c>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -11415,21 +12438,35 @@
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+    <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>545</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>546</v>
+      </c>
       <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
+      <c r="E36" s="35" t="s">
+        <v>560</v>
+      </c>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>540</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>541</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>547</v>
+      </c>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -11437,8 +12474,10 @@
       <c r="H37" s="28"/>
       <c r="I37" s="28"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
+        <v>548</v>
+      </c>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
       <c r="D38" s="28"/>
@@ -11448,49 +12487,408 @@
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="B39" s="35" t="s">
+        <v>554</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>550</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>553</v>
+      </c>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
+      <c r="B40" s="34" t="s">
+        <v>555</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>551</v>
+      </c>
+      <c r="D40" s="34" t="s">
+        <v>557</v>
+      </c>
+      <c r="E40" s="35"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="B41" s="34" t="s">
+        <v>549</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>552</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>556</v>
+      </c>
       <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
+      <c r="F41" s="41" t="s">
+        <v>559</v>
+      </c>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
     </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>561</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>562</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+    </row>
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="42" t="s">
+        <v>563</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>567</v>
+      </c>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>566</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
+        <v>570</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>568</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>572</v>
+      </c>
+      <c r="D45" s="44" t="s">
+        <v>573</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="s">
+        <v>569</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>571</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+    </row>
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
+        <v>574</v>
+      </c>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+    </row>
+    <row r="48" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="B48" s="34" t="s">
+        <v>575</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>579</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>583</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>584</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>585</v>
+      </c>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+    </row>
+    <row r="49" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A49" s="28"/>
+      <c r="B49" s="34" t="s">
+        <v>576</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>580</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>582</v>
+      </c>
+      <c r="E49" s="44" t="s">
+        <v>578</v>
+      </c>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="28"/>
+      <c r="B50" s="34" t="s">
+        <v>577</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>581</v>
+      </c>
+      <c r="D50" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="E50" s="44" t="s">
+        <v>587</v>
+      </c>
+      <c r="F50" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+    </row>
+    <row r="51" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A51" s="44" t="s">
+        <v>589</v>
+      </c>
+      <c r="B51" s="44" t="s">
+        <v>590</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>591</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>593</v>
+      </c>
+      <c r="F51" s="44" t="s">
+        <v>594</v>
+      </c>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+    </row>
+    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="44" t="s">
+        <v>595</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>596</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>597</v>
+      </c>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I20" r:id="rId1" xr:uid="{FA8F7659-D4CE-48A9-9711-2CE212BEF6DF}"/>
+    <hyperlink ref="F41" r:id="rId2" xr:uid="{016A1A40-C028-45CC-BB8F-2558F7DC9819}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>